<commit_message>
Update Evolutionary Computing Sudoku Example.xlsx
</commit_message>
<xml_diff>
--- a/Evolutionary Computing Sudoku Example.xlsx
+++ b/Evolutionary Computing Sudoku Example.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://northeastern-my.sharepoint.com/personal/huebscher_m_northeastern_edu/Documents/Desktop/Stuff/Data Science/Data Science Practice/Sudoku Game/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://northeastern-my.sharepoint.com/personal/huebscher_m_northeastern_edu/Documents/Desktop/Personal GitHub/Sudoku-Solver/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DF50C353-2A20-454E-9CD8-1C31EA447888}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="228" documentId="8_{DF50C353-2A20-454E-9CD8-1C31EA447888}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AB1B8215-7256-429C-B370-42D6F9E188DD}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{D309FC74-AE89-4A55-AE53-4F1BE9C3738B}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{D309FC74-AE89-4A55-AE53-4F1BE9C3738B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="2">
   <si>
     <t>OG Board:</t>
   </si>
@@ -48,7 +48,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -60,6 +60,13 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -220,7 +227,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -250,6 +257,36 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -268,9 +305,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -308,7 +345,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -414,7 +451,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -556,7 +593,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -564,30 +601,33 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B35CBFF5-9B7A-4CFA-AD17-4040B35F1D72}">
-  <dimension ref="C2:K22"/>
+  <dimension ref="C2:V22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" topLeftCell="L1" zoomScale="80" workbookViewId="0">
+      <selection activeCell="P8" sqref="P8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="11" width="5.7109375" customWidth="1"/>
+    <col min="3" max="11" width="5.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="3:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="3:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C2" s="10" t="s">
         <v>0</v>
       </c>
+      <c r="M2" s="10" t="s">
+        <v>0</v>
+      </c>
     </row>
-    <row r="3" spans="3:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="3:22" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C3" s="1">
         <v>6</v>
       </c>
       <c r="D3" s="2">
         <v>3</v>
       </c>
-      <c r="E3" s="3">
+      <c r="E3" s="11">
         <v>0</v>
       </c>
       <c r="F3" s="1">
@@ -608,8 +648,36 @@
       <c r="K3" s="3">
         <v>1</v>
       </c>
+      <c r="M3" s="1">
+        <v>7</v>
+      </c>
+      <c r="N3" s="2">
+        <v>8</v>
+      </c>
+      <c r="O3" s="11">
+        <v>0</v>
+      </c>
+      <c r="P3" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q3" s="2">
+        <v>0</v>
+      </c>
+      <c r="R3" s="3">
+        <v>6</v>
+      </c>
+      <c r="S3" s="1">
+        <v>3</v>
+      </c>
+      <c r="T3" s="2">
+        <v>1</v>
+      </c>
+      <c r="U3" s="3">
+        <v>2</v>
+      </c>
+      <c r="V3" s="19"/>
     </row>
-    <row r="4" spans="3:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="3:22" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C4" s="4">
         <v>8</v>
       </c>
@@ -637,12 +705,40 @@
       <c r="K4" s="6">
         <v>4</v>
       </c>
+      <c r="M4" s="4">
+        <v>2</v>
+      </c>
+      <c r="N4" s="5">
+        <v>6</v>
+      </c>
+      <c r="O4" s="6">
+        <v>4</v>
+      </c>
+      <c r="P4" s="4">
+        <v>1</v>
+      </c>
+      <c r="Q4" s="5">
+        <v>0</v>
+      </c>
+      <c r="R4" s="6">
+        <v>0</v>
+      </c>
+      <c r="S4" s="4">
+        <v>8</v>
+      </c>
+      <c r="T4" s="5">
+        <v>9</v>
+      </c>
+      <c r="U4" s="6">
+        <v>7</v>
+      </c>
+      <c r="V4" s="19"/>
     </row>
-    <row r="5" spans="3:11" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C5" s="7">
-        <v>0</v>
-      </c>
-      <c r="D5" s="8">
+    <row r="5" spans="3:22" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C5" s="12">
+        <v>0</v>
+      </c>
+      <c r="D5" s="13">
         <v>0</v>
       </c>
       <c r="E5" s="9">
@@ -651,7 +747,7 @@
       <c r="F5" s="7">
         <v>8</v>
       </c>
-      <c r="G5" s="8">
+      <c r="G5" s="13">
         <v>0</v>
       </c>
       <c r="H5" s="9">
@@ -663,21 +759,49 @@
       <c r="J5" s="8">
         <v>2</v>
       </c>
-      <c r="K5" s="9">
-        <v>0</v>
-      </c>
+      <c r="K5" s="14">
+        <v>0</v>
+      </c>
+      <c r="M5" s="12">
+        <v>1</v>
+      </c>
+      <c r="N5" s="13">
+        <v>9</v>
+      </c>
+      <c r="O5" s="9">
+        <v>0</v>
+      </c>
+      <c r="P5" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q5" s="13">
+        <v>8</v>
+      </c>
+      <c r="R5" s="9">
+        <v>2</v>
+      </c>
+      <c r="S5" s="7">
+        <v>0</v>
+      </c>
+      <c r="T5" s="8">
+        <v>0</v>
+      </c>
+      <c r="U5" s="14">
+        <v>0</v>
+      </c>
+      <c r="V5" s="20"/>
     </row>
-    <row r="6" spans="3:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="3:22" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C6" s="1">
         <v>4</v>
       </c>
       <c r="D6" s="2">
         <v>8</v>
       </c>
-      <c r="E6" s="3">
-        <v>0</v>
-      </c>
-      <c r="F6" s="1">
+      <c r="E6" s="11">
+        <v>0</v>
+      </c>
+      <c r="F6" s="15">
         <v>0</v>
       </c>
       <c r="G6" s="2">
@@ -689,14 +813,42 @@
       <c r="I6" s="1">
         <v>2</v>
       </c>
-      <c r="J6" s="2">
+      <c r="J6" s="16">
         <v>0</v>
       </c>
       <c r="K6" s="3">
         <v>7</v>
       </c>
+      <c r="M6" s="1">
+        <v>0</v>
+      </c>
+      <c r="N6" s="2">
+        <v>0</v>
+      </c>
+      <c r="O6" s="11">
+        <v>0</v>
+      </c>
+      <c r="P6" s="15">
+        <v>6</v>
+      </c>
+      <c r="Q6" s="2">
+        <v>9</v>
+      </c>
+      <c r="R6" s="3">
+        <v>3</v>
+      </c>
+      <c r="S6" s="1">
+        <v>0</v>
+      </c>
+      <c r="T6" s="16">
+        <v>0</v>
+      </c>
+      <c r="U6" s="3">
+        <v>0</v>
+      </c>
+      <c r="V6" s="19"/>
     </row>
-    <row r="7" spans="3:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="3:22" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C7" s="4">
         <v>7</v>
       </c>
@@ -706,13 +858,13 @@
       <c r="E7" s="6">
         <v>1</v>
       </c>
-      <c r="F7" s="4">
+      <c r="F7" s="18">
         <v>0</v>
       </c>
       <c r="G7" s="5">
         <v>2</v>
       </c>
-      <c r="H7" s="6">
+      <c r="H7" s="17">
         <v>0</v>
       </c>
       <c r="I7" s="4">
@@ -724,12 +876,40 @@
       <c r="K7" s="6">
         <v>9</v>
       </c>
+      <c r="M7" s="4">
+        <v>8</v>
+      </c>
+      <c r="N7" s="5">
+        <v>0</v>
+      </c>
+      <c r="O7" s="6">
+        <v>1</v>
+      </c>
+      <c r="P7" s="18">
+        <v>5</v>
+      </c>
+      <c r="Q7" s="5">
+        <v>0</v>
+      </c>
+      <c r="R7" s="17">
+        <v>0</v>
+      </c>
+      <c r="S7" s="4">
+        <v>0</v>
+      </c>
+      <c r="T7" s="5">
+        <v>0</v>
+      </c>
+      <c r="U7" s="6">
+        <v>0</v>
+      </c>
+      <c r="V7" s="19"/>
     </row>
-    <row r="8" spans="3:11" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="3:22" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C8" s="7">
         <v>2</v>
       </c>
-      <c r="D8" s="8">
+      <c r="D8" s="13">
         <v>0</v>
       </c>
       <c r="E8" s="9">
@@ -741,10 +921,10 @@
       <c r="G8" s="8">
         <v>8</v>
       </c>
-      <c r="H8" s="9">
-        <v>0</v>
-      </c>
-      <c r="I8" s="7">
+      <c r="H8" s="14">
+        <v>0</v>
+      </c>
+      <c r="I8" s="12">
         <v>0</v>
       </c>
       <c r="J8" s="8">
@@ -753,9 +933,37 @@
       <c r="K8" s="9">
         <v>5</v>
       </c>
+      <c r="M8" s="7">
+        <v>0</v>
+      </c>
+      <c r="N8" s="13">
+        <v>5</v>
+      </c>
+      <c r="O8" s="9">
+        <v>6</v>
+      </c>
+      <c r="P8" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q8" s="8">
+        <v>0</v>
+      </c>
+      <c r="R8" s="14">
+        <v>0</v>
+      </c>
+      <c r="S8" s="12">
+        <v>4</v>
+      </c>
+      <c r="T8" s="8">
+        <v>0</v>
+      </c>
+      <c r="U8" s="9">
+        <v>0</v>
+      </c>
+      <c r="V8" s="19"/>
     </row>
-    <row r="9" spans="3:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C9" s="1">
+    <row r="9" spans="3:22" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C9" s="15">
         <v>0</v>
       </c>
       <c r="D9" s="2">
@@ -767,7 +975,7 @@
       <c r="F9" s="1">
         <v>2</v>
       </c>
-      <c r="G9" s="2">
+      <c r="G9" s="16">
         <v>0</v>
       </c>
       <c r="H9" s="3">
@@ -776,14 +984,42 @@
       <c r="I9" s="1">
         <v>9</v>
       </c>
-      <c r="J9" s="2">
-        <v>0</v>
-      </c>
-      <c r="K9" s="3">
-        <v>0</v>
-      </c>
+      <c r="J9" s="16">
+        <v>0</v>
+      </c>
+      <c r="K9" s="11">
+        <v>0</v>
+      </c>
+      <c r="M9" s="15">
+        <v>6</v>
+      </c>
+      <c r="N9" s="2">
+        <v>7</v>
+      </c>
+      <c r="O9" s="3">
+        <v>2</v>
+      </c>
+      <c r="P9" s="1">
+        <v>2</v>
+      </c>
+      <c r="Q9" s="16">
+        <v>0</v>
+      </c>
+      <c r="R9" s="3">
+        <v>9</v>
+      </c>
+      <c r="S9" s="1">
+        <v>0</v>
+      </c>
+      <c r="T9" s="16">
+        <v>0</v>
+      </c>
+      <c r="U9" s="11">
+        <v>4</v>
+      </c>
+      <c r="V9" s="20"/>
     </row>
-    <row r="10" spans="3:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="3:22" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C10" s="4">
         <v>3</v>
       </c>
@@ -811,8 +1047,36 @@
       <c r="K10" s="6">
         <v>2</v>
       </c>
+      <c r="M10" s="4">
+        <v>0</v>
+      </c>
+      <c r="N10" s="5">
+        <v>0</v>
+      </c>
+      <c r="O10" s="6">
+        <v>9</v>
+      </c>
+      <c r="P10" s="4">
+        <v>0</v>
+      </c>
+      <c r="Q10" s="5">
+        <v>0</v>
+      </c>
+      <c r="R10" s="6">
+        <v>0</v>
+      </c>
+      <c r="S10" s="4">
+        <v>7</v>
+      </c>
+      <c r="T10" s="5">
+        <v>3</v>
+      </c>
+      <c r="U10" s="6">
+        <v>1</v>
+      </c>
+      <c r="V10" s="19"/>
     </row>
-    <row r="11" spans="3:11" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="3:22" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C11" s="7">
         <v>9</v>
       </c>
@@ -831,8 +1095,8 @@
       <c r="H11" s="9">
         <v>8</v>
       </c>
-      <c r="I11" s="7">
-        <v>1</v>
+      <c r="I11" s="12">
+        <v>0</v>
       </c>
       <c r="J11" s="8">
         <v>3</v>
@@ -840,21 +1104,52 @@
       <c r="K11" s="9">
         <v>6</v>
       </c>
+      <c r="M11" s="7">
+        <v>0</v>
+      </c>
+      <c r="N11" s="8">
+        <v>0</v>
+      </c>
+      <c r="O11" s="9">
+        <v>0</v>
+      </c>
+      <c r="P11" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q11" s="8">
+        <v>5</v>
+      </c>
+      <c r="R11" s="9">
+        <v>7</v>
+      </c>
+      <c r="S11" s="12">
+        <v>0</v>
+      </c>
+      <c r="T11" s="8">
+        <v>2</v>
+      </c>
+      <c r="U11" s="9">
+        <v>0</v>
+      </c>
+      <c r="V11" s="19"/>
     </row>
-    <row r="13" spans="3:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="3:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C13" s="10" t="s">
         <v>1</v>
       </c>
+      <c r="M13" s="10" t="s">
+        <v>1</v>
+      </c>
     </row>
-    <row r="14" spans="3:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="3:22" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C14" s="1">
         <v>6</v>
       </c>
       <c r="D14" s="2">
         <v>3</v>
       </c>
-      <c r="E14" s="3">
-        <v>0</v>
+      <c r="E14" s="11">
+        <v>9</v>
       </c>
       <c r="F14" s="1">
         <v>5</v>
@@ -874,8 +1169,35 @@
       <c r="K14" s="3">
         <v>1</v>
       </c>
+      <c r="M14" s="1">
+        <v>7</v>
+      </c>
+      <c r="N14" s="2">
+        <v>8</v>
+      </c>
+      <c r="O14" s="11">
+        <v>5</v>
+      </c>
+      <c r="P14" s="1">
+        <v>9</v>
+      </c>
+      <c r="Q14" s="2">
+        <v>4</v>
+      </c>
+      <c r="R14" s="3">
+        <v>6</v>
+      </c>
+      <c r="S14" s="1">
+        <v>3</v>
+      </c>
+      <c r="T14" s="2">
+        <v>1</v>
+      </c>
+      <c r="U14" s="3">
+        <v>2</v>
+      </c>
     </row>
-    <row r="15" spans="3:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="3:22" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C15" s="4">
         <v>8</v>
       </c>
@@ -903,13 +1225,40 @@
       <c r="K15" s="6">
         <v>4</v>
       </c>
+      <c r="M15" s="4">
+        <v>2</v>
+      </c>
+      <c r="N15" s="5">
+        <v>6</v>
+      </c>
+      <c r="O15" s="6">
+        <v>4</v>
+      </c>
+      <c r="P15" s="4">
+        <v>1</v>
+      </c>
+      <c r="Q15" s="5">
+        <v>3</v>
+      </c>
+      <c r="R15" s="6">
+        <v>5</v>
+      </c>
+      <c r="S15" s="4">
+        <v>8</v>
+      </c>
+      <c r="T15" s="5">
+        <v>9</v>
+      </c>
+      <c r="U15" s="6">
+        <v>7</v>
+      </c>
     </row>
-    <row r="16" spans="3:11" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C16" s="7">
-        <v>0</v>
-      </c>
-      <c r="D16" s="8">
-        <v>0</v>
+    <row r="16" spans="3:22" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C16" s="12">
+        <v>5</v>
+      </c>
+      <c r="D16" s="13">
+        <v>4</v>
       </c>
       <c r="E16" s="9">
         <v>7</v>
@@ -917,8 +1266,8 @@
       <c r="F16" s="7">
         <v>8</v>
       </c>
-      <c r="G16" s="8">
-        <v>0</v>
+      <c r="G16" s="13">
+        <v>1</v>
       </c>
       <c r="H16" s="9">
         <v>9</v>
@@ -929,22 +1278,49 @@
       <c r="J16" s="8">
         <v>2</v>
       </c>
-      <c r="K16" s="9">
-        <v>0</v>
+      <c r="K16" s="14">
+        <v>3</v>
+      </c>
+      <c r="M16" s="12">
+        <v>1</v>
+      </c>
+      <c r="N16" s="13">
+        <v>9</v>
+      </c>
+      <c r="O16" s="9">
+        <v>3</v>
+      </c>
+      <c r="P16" s="7">
+        <v>7</v>
+      </c>
+      <c r="Q16" s="13">
+        <v>8</v>
+      </c>
+      <c r="R16" s="9">
+        <v>2</v>
+      </c>
+      <c r="S16" s="7">
+        <v>6</v>
+      </c>
+      <c r="T16" s="8">
+        <v>4</v>
+      </c>
+      <c r="U16" s="14">
+        <v>5</v>
       </c>
     </row>
-    <row r="17" spans="3:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="3:21" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C17" s="1">
         <v>4</v>
       </c>
       <c r="D17" s="2">
         <v>8</v>
       </c>
-      <c r="E17" s="3">
-        <v>0</v>
-      </c>
-      <c r="F17" s="1">
-        <v>0</v>
+      <c r="E17" s="11">
+        <v>3</v>
+      </c>
+      <c r="F17" s="15">
+        <v>1</v>
       </c>
       <c r="G17" s="2">
         <v>9</v>
@@ -955,14 +1331,41 @@
       <c r="I17" s="1">
         <v>2</v>
       </c>
-      <c r="J17" s="2">
-        <v>0</v>
+      <c r="J17" s="16">
+        <v>6</v>
       </c>
       <c r="K17" s="3">
         <v>7</v>
       </c>
+      <c r="M17" s="1">
+        <v>4</v>
+      </c>
+      <c r="N17" s="2">
+        <v>2</v>
+      </c>
+      <c r="O17" s="11">
+        <v>7</v>
+      </c>
+      <c r="P17" s="15">
+        <v>6</v>
+      </c>
+      <c r="Q17" s="2">
+        <v>9</v>
+      </c>
+      <c r="R17" s="3">
+        <v>3</v>
+      </c>
+      <c r="S17" s="1">
+        <v>1</v>
+      </c>
+      <c r="T17" s="16">
+        <v>5</v>
+      </c>
+      <c r="U17" s="3">
+        <v>8</v>
+      </c>
     </row>
-    <row r="18" spans="3:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="3:21" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C18" s="4">
         <v>7</v>
       </c>
@@ -972,14 +1375,14 @@
       <c r="E18" s="6">
         <v>1</v>
       </c>
-      <c r="F18" s="4">
-        <v>0</v>
+      <c r="F18" s="18">
+        <v>6</v>
       </c>
       <c r="G18" s="5">
         <v>2</v>
       </c>
-      <c r="H18" s="6">
-        <v>0</v>
+      <c r="H18" s="17">
+        <v>3</v>
       </c>
       <c r="I18" s="4">
         <v>8</v>
@@ -990,13 +1393,40 @@
       <c r="K18" s="6">
         <v>9</v>
       </c>
+      <c r="M18" s="4">
+        <v>8</v>
+      </c>
+      <c r="N18" s="5">
+        <v>3</v>
+      </c>
+      <c r="O18" s="6">
+        <v>1</v>
+      </c>
+      <c r="P18" s="18">
+        <v>5</v>
+      </c>
+      <c r="Q18" s="5">
+        <v>7</v>
+      </c>
+      <c r="R18" s="17">
+        <v>4</v>
+      </c>
+      <c r="S18" s="4">
+        <v>2</v>
+      </c>
+      <c r="T18" s="5">
+        <v>6</v>
+      </c>
+      <c r="U18" s="6">
+        <v>9</v>
+      </c>
     </row>
-    <row r="19" spans="3:11" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="3:21" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C19" s="7">
         <v>2</v>
       </c>
-      <c r="D19" s="8">
-        <v>0</v>
+      <c r="D19" s="13">
+        <v>9</v>
       </c>
       <c r="E19" s="9">
         <v>6</v>
@@ -1007,11 +1437,11 @@
       <c r="G19" s="8">
         <v>8</v>
       </c>
-      <c r="H19" s="9">
-        <v>0</v>
-      </c>
-      <c r="I19" s="7">
-        <v>0</v>
+      <c r="H19" s="14">
+        <v>4</v>
+      </c>
+      <c r="I19" s="12">
+        <v>3</v>
       </c>
       <c r="J19" s="8">
         <v>1</v>
@@ -1019,10 +1449,37 @@
       <c r="K19" s="9">
         <v>5</v>
       </c>
+      <c r="M19" s="7">
+        <v>9</v>
+      </c>
+      <c r="N19" s="13">
+        <v>5</v>
+      </c>
+      <c r="O19" s="9">
+        <v>6</v>
+      </c>
+      <c r="P19" s="7">
+        <v>8</v>
+      </c>
+      <c r="Q19" s="8">
+        <v>2</v>
+      </c>
+      <c r="R19" s="14">
+        <v>1</v>
+      </c>
+      <c r="S19" s="12">
+        <v>4</v>
+      </c>
+      <c r="T19" s="8">
+        <v>7</v>
+      </c>
+      <c r="U19" s="9">
+        <v>3</v>
+      </c>
     </row>
-    <row r="20" spans="3:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C20" s="1">
-        <v>0</v>
+    <row r="20" spans="3:21" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C20" s="15">
+        <v>1</v>
       </c>
       <c r="D20" s="2">
         <v>7</v>
@@ -1033,8 +1490,8 @@
       <c r="F20" s="1">
         <v>2</v>
       </c>
-      <c r="G20" s="2">
-        <v>0</v>
+      <c r="G20" s="16">
+        <v>3</v>
       </c>
       <c r="H20" s="3">
         <v>6</v>
@@ -1042,14 +1499,41 @@
       <c r="I20" s="1">
         <v>9</v>
       </c>
-      <c r="J20" s="2">
-        <v>0</v>
-      </c>
-      <c r="K20" s="3">
-        <v>0</v>
+      <c r="J20" s="16">
+        <v>5</v>
+      </c>
+      <c r="K20" s="11">
+        <v>8</v>
+      </c>
+      <c r="M20" s="15">
+        <v>6</v>
+      </c>
+      <c r="N20" s="2">
+        <v>7</v>
+      </c>
+      <c r="O20" s="3">
+        <v>2</v>
+      </c>
+      <c r="P20" s="1">
+        <v>3</v>
+      </c>
+      <c r="Q20" s="16">
+        <v>1</v>
+      </c>
+      <c r="R20" s="3">
+        <v>9</v>
+      </c>
+      <c r="S20" s="1">
+        <v>5</v>
+      </c>
+      <c r="T20" s="16">
+        <v>8</v>
+      </c>
+      <c r="U20" s="11">
+        <v>4</v>
       </c>
     </row>
-    <row r="21" spans="3:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="3:21" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C21" s="4">
         <v>3</v>
       </c>
@@ -1077,8 +1561,35 @@
       <c r="K21" s="6">
         <v>2</v>
       </c>
+      <c r="M21" s="4">
+        <v>5</v>
+      </c>
+      <c r="N21" s="5">
+        <v>4</v>
+      </c>
+      <c r="O21" s="6">
+        <v>9</v>
+      </c>
+      <c r="P21" s="4">
+        <v>2</v>
+      </c>
+      <c r="Q21" s="5">
+        <v>6</v>
+      </c>
+      <c r="R21" s="6">
+        <v>8</v>
+      </c>
+      <c r="S21" s="4">
+        <v>7</v>
+      </c>
+      <c r="T21" s="5">
+        <v>3</v>
+      </c>
+      <c r="U21" s="6">
+        <v>1</v>
+      </c>
     </row>
-    <row r="22" spans="3:11" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="3:21" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C22" s="7">
         <v>9</v>
       </c>
@@ -1097,13 +1608,40 @@
       <c r="H22" s="9">
         <v>8</v>
       </c>
-      <c r="I22" s="7">
+      <c r="I22" s="12">
         <v>1</v>
       </c>
       <c r="J22" s="8">
         <v>3</v>
       </c>
       <c r="K22" s="9">
+        <v>6</v>
+      </c>
+      <c r="M22" s="7">
+        <v>3</v>
+      </c>
+      <c r="N22" s="8">
+        <v>1</v>
+      </c>
+      <c r="O22" s="9">
+        <v>8</v>
+      </c>
+      <c r="P22" s="7">
+        <v>4</v>
+      </c>
+      <c r="Q22" s="8">
+        <v>5</v>
+      </c>
+      <c r="R22" s="9">
+        <v>7</v>
+      </c>
+      <c r="S22" s="12">
+        <v>9</v>
+      </c>
+      <c r="T22" s="8">
+        <v>2</v>
+      </c>
+      <c r="U22" s="9">
         <v>6</v>
       </c>
     </row>
@@ -1355,20 +1893,20 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="7c9f12b8-e948-49f0-9fa4-6dfb96355127" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="7c9f12b8-e948-49f0-9fa4-6dfb96355127" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1391,26 +1929,19 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{52788784-EA7E-4CA9-9829-DAF629900478}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="7c9f12b8-e948-49f0-9fa4-6dfb96355127"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{204A00A1-345B-40F8-A296-81CE2C8420CB}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{52788784-EA7E-4CA9-9829-DAF629900478}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="4bd4e26f-3f74-4ddd-9d59-410bca28f133"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="7c9f12b8-e948-49f0-9fa4-6dfb96355127"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>